<commit_message>
aggiornata verifica dei requisiti
</commit_message>
<xml_diff>
--- a/RR/Esterni/Piano di qualifica/VerificaRequisiti.xlsx
+++ b/RR/Esterni/Piano di qualifica/VerificaRequisiti.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="317">
   <si>
     <t>Test</t>
   </si>
@@ -58,33 +58,6 @@
     <t>Viene verificato che l'amministratore possa eliminare un template</t>
   </si>
   <si>
-    <t>Viene verificato che l'amministratore possa modificare un template</t>
-  </si>
-  <si>
-    <t>Viene verificato che l'amministratore possa inserire un nuovo elemento nel template</t>
-  </si>
-  <si>
-    <t>Viene verificato che l'ammistratore possa modificare la dimensione di un elemento grafico del template</t>
-  </si>
-  <si>
-    <t>Viene verificato che l'amministratore possa modificare lo sfondo di un template</t>
-  </si>
-  <si>
-    <t>Viene verificato che l'amministratore possa modificare un elemento testuale di un template</t>
-  </si>
-  <si>
-    <t>Viene verificato che l'amministratore possa eliminare un elemento presente in un template</t>
-  </si>
-  <si>
-    <t>Viene verificato che l'amministratore possa annullare l'ultima modifica apportata</t>
-  </si>
-  <si>
-    <t>Viene verificato che l'amministratore possa ripristinare lo stato di un template prima dell'inizio delle operazioni di modifica</t>
-  </si>
-  <si>
-    <t>Viene verificato che l'amministratore possa ripristinare un template appena eliminato</t>
-  </si>
-  <si>
     <t>TS1</t>
   </si>
   <si>
@@ -100,15 +73,6 @@
     <t>Viene verificato che si possa creare una nuova presentazione vuota</t>
   </si>
   <si>
-    <t>Viene verificato che si possa passare in modalità modifica di una presentazione</t>
-  </si>
-  <si>
-    <t>TS7.1</t>
-  </si>
-  <si>
-    <t>RF7.1</t>
-  </si>
-  <si>
     <t>TS7.1.1</t>
   </si>
   <si>
@@ -118,69 +82,12 @@
     <t>Viene verificato che si possa scegliere il tipo di frame da inserire</t>
   </si>
   <si>
-    <t>TS7.4</t>
-  </si>
-  <si>
-    <t>RF7.4</t>
-  </si>
-  <si>
-    <t>Viene verificato che si possa inserire un nuovo frame in modalità modifica</t>
-  </si>
-  <si>
     <t>Viene verificato che si possa spostare un frame in modalità modifica</t>
   </si>
   <si>
-    <t>TS7.7</t>
-  </si>
-  <si>
-    <t>RF7.7</t>
-  </si>
-  <si>
     <t>Viene verificato che si possa passare in modalità modifica di un frame</t>
   </si>
   <si>
-    <t>TS7.7.1</t>
-  </si>
-  <si>
-    <t>RF7.7.1</t>
-  </si>
-  <si>
-    <t>TS7.7.4</t>
-  </si>
-  <si>
-    <t>TS7.7.7</t>
-  </si>
-  <si>
-    <t>TS7.7.10</t>
-  </si>
-  <si>
-    <t>TS7.7.19</t>
-  </si>
-  <si>
-    <t>TS7.7.22</t>
-  </si>
-  <si>
-    <t>TS7.7.25</t>
-  </si>
-  <si>
-    <t>RF7.7.4</t>
-  </si>
-  <si>
-    <t>RF7.7.7</t>
-  </si>
-  <si>
-    <t>RF7.7.10</t>
-  </si>
-  <si>
-    <t>RF7.7.19</t>
-  </si>
-  <si>
-    <t>RF7.7.22</t>
-  </si>
-  <si>
-    <t>RF7.7.25</t>
-  </si>
-  <si>
     <t>Viene verificato che si possa inserire un immagine all'interno del frame</t>
   </si>
   <si>
@@ -199,21 +106,6 @@
     <t>Viene verificato che si possa eliminare un elemento presente all'interno del frame</t>
   </si>
   <si>
-    <t>TS7.7.28</t>
-  </si>
-  <si>
-    <t>TS7.7.31</t>
-  </si>
-  <si>
-    <t>TS7.7.40</t>
-  </si>
-  <si>
-    <t>RF7.7.28</t>
-  </si>
-  <si>
-    <t>RF7.7.31</t>
-  </si>
-  <si>
     <t>Verificare che si possa modificare il testo di un elemento scelta</t>
   </si>
   <si>
@@ -226,40 +118,6 @@
     <t>Viene verificato che si possa modificare lo sfondo di un frame</t>
   </si>
   <si>
-    <t>RF7.7.40
-RF7.7.43</t>
-  </si>
-  <si>
-    <t>TS7.10</t>
-  </si>
-  <si>
-    <t>RF7.10</t>
-  </si>
-  <si>
-    <t>TS7.13</t>
-  </si>
-  <si>
-    <t>TS7.16</t>
-  </si>
-  <si>
-    <t>TS7.19</t>
-  </si>
-  <si>
-    <t>TS7.19.1</t>
-  </si>
-  <si>
-    <t>RF7.13</t>
-  </si>
-  <si>
-    <t>RF7.16</t>
-  </si>
-  <si>
-    <t>RF7.19</t>
-  </si>
-  <si>
-    <t>RF7.19.1</t>
-  </si>
-  <si>
     <t>Viene verificato che si possa eliminare un frame dal piano di una presentazione</t>
   </si>
   <si>
@@ -275,30 +133,6 @@
     <t>Viene verificato che si possa impostare un frame iniziale per il percorso di presentazione</t>
   </si>
   <si>
-    <t>TS7.19.4</t>
-  </si>
-  <si>
-    <t>TS7.19.7</t>
-  </si>
-  <si>
-    <t>TS7.19.10</t>
-  </si>
-  <si>
-    <t>TS7.19.13</t>
-  </si>
-  <si>
-    <t>RF7.19.4</t>
-  </si>
-  <si>
-    <t>RF7.19.7</t>
-  </si>
-  <si>
-    <t>RF7.19.10</t>
-  </si>
-  <si>
-    <t>RF7.19.13</t>
-  </si>
-  <si>
     <t>Viene verificato che si possa definire una transizione tra due frame</t>
   </si>
   <si>
@@ -311,33 +145,12 @@
     <t>Viene verificato che si possa togliere un frame dal percorso di presentazione</t>
   </si>
   <si>
-    <t>TS7.22</t>
-  </si>
-  <si>
-    <t>RF7.22</t>
-  </si>
-  <si>
-    <t>TS7.25</t>
-  </si>
-  <si>
-    <t>TS7.37</t>
-  </si>
-  <si>
-    <t>RF7.25</t>
-  </si>
-  <si>
-    <t>RF7.37</t>
-  </si>
-  <si>
     <t>Viene verificato che si possa assegnare un bookmark ad un frame</t>
   </si>
   <si>
     <t>Viene verificato che si possa rimuovere un bookmark da un frame</t>
   </si>
   <si>
-    <t>Viene verificato che si possa salvare la presentazione in una cartella locale all'applicazione</t>
-  </si>
-  <si>
     <t>TS10</t>
   </si>
   <si>
@@ -392,60 +205,18 @@
     <t>Viene verificato che si possa rimuover un bookmark ad un frame da mobile</t>
   </si>
   <si>
-    <t>TS7.7.13</t>
-  </si>
-  <si>
-    <t>TS7.7.16</t>
-  </si>
-  <si>
-    <t>RF7.7.13</t>
-  </si>
-  <si>
-    <t>RF7.7.16</t>
-  </si>
-  <si>
     <t>Viene verificato che si possa inserire un video all'interno di un frame</t>
   </si>
   <si>
     <t>Viene verificato che si possa modificare la dimensione di un video all'interno di un frame</t>
   </si>
   <si>
-    <t>TS7.7.34</t>
-  </si>
-  <si>
-    <t>TS7.7.37</t>
-  </si>
-  <si>
-    <t>RF7.7.34</t>
-  </si>
-  <si>
-    <t>RF7.7.37</t>
-  </si>
-  <si>
     <t>Viene verificato che si possa modificare lo spessore del bordo di un frame</t>
   </si>
   <si>
     <t>Viene verificato che si possa modificare il colore del bordo di un frame</t>
   </si>
   <si>
-    <t>TS7.28</t>
-  </si>
-  <si>
-    <t>TS7.31</t>
-  </si>
-  <si>
-    <t>TS7.34</t>
-  </si>
-  <si>
-    <t>RF7.28</t>
-  </si>
-  <si>
-    <t>RF7.31</t>
-  </si>
-  <si>
-    <t>RF7.34</t>
-  </si>
-  <si>
     <t>Viene verificato che si possa modificare la velocità di transizione tra due frame consecutivi</t>
   </si>
   <si>
@@ -470,9 +241,6 @@
     <t>TS25</t>
   </si>
   <si>
-    <t>TS28</t>
-  </si>
-  <si>
     <t>TS31</t>
   </si>
   <si>
@@ -482,9 +250,6 @@
     <t>TS37</t>
   </si>
   <si>
-    <t>TS40</t>
-  </si>
-  <si>
     <t>RF16</t>
   </si>
   <si>
@@ -494,9 +259,6 @@
     <t>RF25</t>
   </si>
   <si>
-    <t>RF28</t>
-  </si>
-  <si>
     <t>RF31</t>
   </si>
   <si>
@@ -506,24 +268,9 @@
     <t>RF37</t>
   </si>
   <si>
-    <t>RF40</t>
-  </si>
-  <si>
-    <t>Viene verificato che all'interno dello spazio dell'utente nel server ci siano 3 cartelle diverse contenenti rispettivamente presentazioni, infografiche ed immagini</t>
-  </si>
-  <si>
     <t>Viene verificato che si possa caricare un immagine dal proprio File System alla propria parte dedicata alle immagini</t>
   </si>
   <si>
-    <t>Viene verificato che si possa creare una nuova cartella all'interno del proprio spazio sul server</t>
-  </si>
-  <si>
-    <t>Viene verificato che si possano spostare le proprie presentazioni all'interno  della cartella dedicata sul suo spazio sul server</t>
-  </si>
-  <si>
-    <t>Viene verificato che si possano spostare le proprie immagini caricate all'interno della cartella dedicata sul suo spazio server</t>
-  </si>
-  <si>
     <t>Viene verificato che si possano spostare le proprie infografiche all'interno della cartella dedicata sul server</t>
   </si>
   <si>
@@ -533,9 +280,6 @@
     <t>Viene verificato che si possa eliminare dal server un'infografica creata</t>
   </si>
   <si>
-    <t>Viene verificato che si possa eliminare dal server un'immagine caricata</t>
-  </si>
-  <si>
     <t>TS43</t>
   </si>
   <si>
@@ -602,18 +346,6 @@
     <t>RF61.1.1</t>
   </si>
   <si>
-    <t>TS61.1.2</t>
-  </si>
-  <si>
-    <t>RF61.1.2</t>
-  </si>
-  <si>
-    <t>TS61.1.3</t>
-  </si>
-  <si>
-    <t>RF61.1.3</t>
-  </si>
-  <si>
     <t>TS61.1.4</t>
   </si>
   <si>
@@ -623,63 +355,18 @@
     <t>Viene verificato che si possa passare da un frame visualizzato al suo frame contenitore</t>
   </si>
   <si>
-    <t>TS61.1.5</t>
-  </si>
-  <si>
-    <t>RF61.1.5</t>
-  </si>
-  <si>
-    <t>TS61.1.6.1</t>
-  </si>
-  <si>
-    <t>RF61.1.6.1</t>
-  </si>
-  <si>
-    <t>TS61.1.6.2</t>
-  </si>
-  <si>
-    <t>RF61.1.6.2</t>
-  </si>
-  <si>
-    <t>TS61.1.6.3</t>
-  </si>
-  <si>
-    <t>RF61.1.6.3</t>
-  </si>
-  <si>
     <t>Viene verificato che si possa eseguire un video da un punto qualsiasi dello stesso</t>
   </si>
   <si>
-    <t>TS61.1.6.4</t>
-  </si>
-  <si>
-    <t>RF61.1.6.4</t>
-  </si>
-  <si>
     <t>Viene verificato che si possa interrompere l'esecuzione di un video</t>
   </si>
   <si>
     <t>RF64</t>
   </si>
   <si>
-    <t>TS61.3</t>
-  </si>
-  <si>
-    <t>TS61.3.1</t>
-  </si>
-  <si>
-    <t>TS61.3.2</t>
-  </si>
-  <si>
-    <t>TS61.3.3</t>
-  </si>
-  <si>
     <t>Viene verificato che si possa eseguire una presentazione in modalità automatica</t>
   </si>
   <si>
-    <t>RF61.3</t>
-  </si>
-  <si>
     <t>Viene verificato che si possa chiudere una presentazione in esecuzione automatica</t>
   </si>
   <si>
@@ -692,28 +379,12 @@
     <t>TS61.4</t>
   </si>
   <si>
-    <t>RF61.3.1</t>
-  </si>
-  <si>
-    <t>RF61.3.2</t>
-  </si>
-  <si>
-    <t>RF61.3.3</t>
-  </si>
-  <si>
     <t>Viene verificato che si possa passare da presentazione automatica a presentazione manuale e viceversa</t>
   </si>
   <si>
-    <t>RF61.4
-RF61.5</t>
-  </si>
-  <si>
     <t>TS64</t>
   </si>
   <si>
-    <t>Viene verificato che si possa effettuare il logout dal server e passare alla modalità offline</t>
-  </si>
-  <si>
     <t>TS67.1</t>
   </si>
   <si>
@@ -732,30 +403,6 @@
     <t>RF67.13</t>
   </si>
   <si>
-    <t>RF67.13.1</t>
-  </si>
-  <si>
-    <t>RF67.13.4</t>
-  </si>
-  <si>
-    <t>RF67.13.7</t>
-  </si>
-  <si>
-    <t>RF67.13.10</t>
-  </si>
-  <si>
-    <t>RF67.13.13</t>
-  </si>
-  <si>
-    <t>RF67.16</t>
-  </si>
-  <si>
-    <t>RF67.19</t>
-  </si>
-  <si>
-    <t>RF67.22</t>
-  </si>
-  <si>
     <t>TS67.4</t>
   </si>
   <si>
@@ -768,35 +415,567 @@
     <t>TS67.13</t>
   </si>
   <si>
-    <t>TS67.13.1</t>
-  </si>
-  <si>
-    <t>TS67.13.4</t>
-  </si>
-  <si>
-    <t>TS67.13.7</t>
-  </si>
-  <si>
-    <t>TS67.13.10</t>
-  </si>
-  <si>
-    <t>TS67.13.13</t>
-  </si>
-  <si>
-    <t>TS67.16</t>
-  </si>
-  <si>
-    <t>TS67.19</t>
-  </si>
-  <si>
-    <t>TS67.22</t>
+    <t>Viene verificato che ci si possa registrare al sistema inserendo username e password</t>
+  </si>
+  <si>
+    <t>TS3</t>
+  </si>
+  <si>
+    <t>RF3</t>
+  </si>
+  <si>
+    <t>Viene verificato che ci si possa autenticare con username e password</t>
+  </si>
+  <si>
+    <t>RF4</t>
+  </si>
+  <si>
+    <t>TS4</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa inserire un nuovo frame nel piano della presentazione</t>
+  </si>
+  <si>
+    <t>TS7.1.1.1</t>
+  </si>
+  <si>
+    <t>RF7.1.1.1</t>
+  </si>
+  <si>
+    <t>TS7.1.4</t>
+  </si>
+  <si>
+    <t>RF7.1.4</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa passare in modalità modifica di una presentazione da desktop</t>
+  </si>
+  <si>
+    <t>TS7.1.7</t>
+  </si>
+  <si>
+    <t>RF7.1.7</t>
+  </si>
+  <si>
+    <t>TS7.1.7.1</t>
+  </si>
+  <si>
+    <t>RF7.1.7.1</t>
+  </si>
+  <si>
+    <t>TS7.1.7.4</t>
+  </si>
+  <si>
+    <t>RF7.1.7.4</t>
+  </si>
+  <si>
+    <t>TS7.1.7.7</t>
+  </si>
+  <si>
+    <t>RF7.1.7.7</t>
+  </si>
+  <si>
+    <t>TS7.1.7.10</t>
+  </si>
+  <si>
+    <t>RF7.1.7.10</t>
+  </si>
+  <si>
+    <t>TS7.1.7.13</t>
+  </si>
+  <si>
+    <t>RF7.1.7.13</t>
+  </si>
+  <si>
+    <t>TS7.1.7.16</t>
+  </si>
+  <si>
+    <t>RF7.1.7.16</t>
+  </si>
+  <si>
+    <t>TS7.1.7.19</t>
+  </si>
+  <si>
+    <t>RF7.1.7.19</t>
+  </si>
+  <si>
+    <t>TS7.1.7.22</t>
+  </si>
+  <si>
+    <t>RF7.1.7.22</t>
+  </si>
+  <si>
+    <t>TS7.1.7.25</t>
+  </si>
+  <si>
+    <t>RF7.1.7.25</t>
+  </si>
+  <si>
+    <t>TS7.1.7.28</t>
+  </si>
+  <si>
+    <t>RF7.1.7.28</t>
+  </si>
+  <si>
+    <t>TS7.1.7.31</t>
+  </si>
+  <si>
+    <t>RF7.1.7.31</t>
+  </si>
+  <si>
+    <t>TS7.1.7.34</t>
+  </si>
+  <si>
+    <t>RF7.1.7.34</t>
+  </si>
+  <si>
+    <t>TS7.1.7.37</t>
+  </si>
+  <si>
+    <t>RF7.1.7.37</t>
+  </si>
+  <si>
+    <t>TS7.1.7.40</t>
+  </si>
+  <si>
+    <t>RF7.1.7.40
+RF7.1.7.43</t>
+  </si>
+  <si>
+    <t>TS7.1.10</t>
+  </si>
+  <si>
+    <t>RF7.1.10</t>
+  </si>
+  <si>
+    <t>TS7.1.13</t>
+  </si>
+  <si>
+    <t>RF7.1.13</t>
+  </si>
+  <si>
+    <t>TS7.1.16</t>
+  </si>
+  <si>
+    <t>RF7.1.16</t>
+  </si>
+  <si>
+    <t>TS7.1.19</t>
+  </si>
+  <si>
+    <t>RF7.1.19</t>
+  </si>
+  <si>
+    <t>TS7.1.19.1</t>
+  </si>
+  <si>
+    <t>RF7.1.19.1</t>
+  </si>
+  <si>
+    <t>TS7.1.19.4</t>
+  </si>
+  <si>
+    <t>RF7.1.19.4</t>
+  </si>
+  <si>
+    <t>TS7.1.19.7</t>
+  </si>
+  <si>
+    <t>RF7.1.19.7</t>
+  </si>
+  <si>
+    <t>TS7.1.19.10</t>
+  </si>
+  <si>
+    <t>RF7.1.19.10</t>
+  </si>
+  <si>
+    <t>TS7.1.19.13</t>
+  </si>
+  <si>
+    <t>RF7.1.19.13</t>
+  </si>
+  <si>
+    <t>TS7.1.22</t>
+  </si>
+  <si>
+    <t>RF7.1.22</t>
+  </si>
+  <si>
+    <t>TS7.1.25</t>
+  </si>
+  <si>
+    <t>RF7.1.25</t>
+  </si>
+  <si>
+    <t>TS7.1.28</t>
+  </si>
+  <si>
+    <t>RF7.1.28</t>
+  </si>
+  <si>
+    <t>TS7.1.31</t>
+  </si>
+  <si>
+    <t>RF7.1.31</t>
+  </si>
+  <si>
+    <t>TS7.1.34</t>
+  </si>
+  <si>
+    <t>RF7.1.34</t>
+  </si>
+  <si>
+    <t>TS7.1.37</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa annullare e ripristinare una modifica appena effettuata</t>
+  </si>
+  <si>
+    <t>RF7.1.37
+RF7.1.40</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possano eliminare dal server le immagini caricate</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa creare nuove cartelle e spostare i file all'interno delle cartelle</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possano organizzare le proprie presentazione con una struttura a cartelle</t>
+  </si>
+  <si>
+    <t>TS61.1.7</t>
+  </si>
+  <si>
+    <t>RF61.1.7</t>
+  </si>
+  <si>
+    <t>TS61.1.10</t>
+  </si>
+  <si>
+    <t>RF61.1.10</t>
+  </si>
+  <si>
+    <t>TS61.1.13</t>
+  </si>
+  <si>
+    <t>RF61.1.13</t>
+  </si>
+  <si>
+    <t>TS61.1.16.1</t>
+  </si>
+  <si>
+    <t>RF61.1.16.1</t>
+  </si>
+  <si>
+    <t>TS61.1.16.4</t>
+  </si>
+  <si>
+    <t>RF61.1.16.4</t>
+  </si>
+  <si>
+    <t>TS61.1.16.7</t>
+  </si>
+  <si>
+    <t>RF61.1.16.7</t>
+  </si>
+  <si>
+    <t>TS61.1.16.10</t>
+  </si>
+  <si>
+    <t>RF61.1.16.10</t>
+  </si>
+  <si>
+    <t>RF61.4</t>
+  </si>
+  <si>
+    <t>TS61.4.1</t>
+  </si>
+  <si>
+    <t>RF61.4.1</t>
+  </si>
+  <si>
+    <t>TS61.4.4</t>
+  </si>
+  <si>
+    <t>RF61.4.4</t>
+  </si>
+  <si>
+    <t>TS61.4.7</t>
+  </si>
+  <si>
+    <t>RF61.4.7</t>
+  </si>
+  <si>
+    <t>TS61.4.10</t>
+  </si>
+  <si>
+    <t>RF61.4.10</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa saltare la riproduzione di un video nel frame visualizzato</t>
+  </si>
+  <si>
+    <t>TS61.7</t>
+  </si>
+  <si>
+    <t>RF61.7
+RF61.10</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa effettuare il logout dal server</t>
+  </si>
+  <si>
+    <t>Viene verificato che l'amministratore possa annullare l'ultima eliminazione di un template</t>
+  </si>
+  <si>
+    <t>TS70.1</t>
+  </si>
+  <si>
+    <t>RF70.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viene verificato che si possa selezionare una presentazione da cui produrre l'infografica </t>
+  </si>
+  <si>
+    <t>TS70.4</t>
+  </si>
+  <si>
+    <t>RF70.4</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa selezionare template di infografica</t>
+  </si>
+  <si>
+    <t>TS70.7</t>
+  </si>
+  <si>
+    <t>RF70.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viene verificato che si possano selezionare gli elementi del </t>
+  </si>
+  <si>
+    <t>TS70.10</t>
+  </si>
+  <si>
+    <t>RF70.10</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa passare in modalità modifica di un'infografica</t>
+  </si>
+  <si>
+    <t>TS70.10.1</t>
+  </si>
+  <si>
+    <t>RF70.10.1</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa modificare un elemento di un infografica</t>
+  </si>
+  <si>
+    <t>TS70.10.1.1</t>
+  </si>
+  <si>
+    <t>RF70.10.1.1</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possano modificare le dimensioni di un immagine</t>
+  </si>
+  <si>
+    <t>TS70.10.1.4</t>
+  </si>
+  <si>
+    <t>RF70.10.1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viene verificato che si possa modificare un elemento testo </t>
+  </si>
+  <si>
+    <t>TS70.10.1.4.1</t>
+  </si>
+  <si>
+    <t>RF70.10.1.4.1</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa modificare il font del testo</t>
+  </si>
+  <si>
+    <t>TS70.10.1.4.4</t>
+  </si>
+  <si>
+    <t>RF70.10.1.4.4</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa modificare la dimensione del carattere</t>
+  </si>
+  <si>
+    <t>TS70.10.1.4.7</t>
+  </si>
+  <si>
+    <t>RF70.10.1.4.7</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa modificare lo stile del testo</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa modificare il colore della scritta del testo</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa modicare il colore dell'evidenziazione del testo</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa cambiare la posizione dell'elemento</t>
+  </si>
+  <si>
+    <t>TS70.10.1.4.10</t>
+  </si>
+  <si>
+    <t>RF70.10.1.4.10</t>
+  </si>
+  <si>
+    <t>RF70.10.1.4.13</t>
+  </si>
+  <si>
+    <t>TS70.10.1.4.13</t>
+  </si>
+  <si>
+    <t>RF70.4.4</t>
+  </si>
+  <si>
+    <t>TS70.10.1.7</t>
+  </si>
+  <si>
+    <t>RF70.10.1.7</t>
+  </si>
+  <si>
+    <t>TS70.10.4</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa rimuover lo sfondo dell'infografica</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa inserire uno sfondo nell'infografica</t>
+  </si>
+  <si>
+    <t>TS70.10.10</t>
+  </si>
+  <si>
+    <t>TS70.10.7</t>
+  </si>
+  <si>
+    <t>RF70.10.7</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa inserire un elemento immagine nell'infografica</t>
+  </si>
+  <si>
+    <t>RF70.10.10</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa inserire del testo nell'infografica</t>
+  </si>
+  <si>
+    <t>TS70.10.13</t>
+  </si>
+  <si>
+    <t>RF70.10.13</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa inserire un frame nella sua interezza presente nella presentazione</t>
+  </si>
+  <si>
+    <t>TS70.10.16</t>
+  </si>
+  <si>
+    <t>RF70.10.16</t>
+  </si>
+  <si>
+    <t>TS70.10.19</t>
+  </si>
+  <si>
+    <t>RF70.10.19</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possano eliminare elementi immagini o testuali</t>
+  </si>
+  <si>
+    <t>TS70.13</t>
+  </si>
+  <si>
+    <t>RF70.13</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa salvare l'infografica nel suo spazio</t>
+  </si>
+  <si>
+    <t>TS70.16</t>
+  </si>
+  <si>
+    <t>RF70.16</t>
+  </si>
+  <si>
+    <t>TS70.19</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa esportare un'infografica in formato stampabile</t>
+  </si>
+  <si>
+    <t>TS73</t>
+  </si>
+  <si>
+    <t>Viene verificato che si possa creare un'infografica</t>
+  </si>
+  <si>
+    <t>RF73</t>
+  </si>
+  <si>
+    <t>RF70.19</t>
+  </si>
+  <si>
+    <t>Viene verificato che ogni funzionalità dell'applicazione sia documentato</t>
+  </si>
+  <si>
+    <t>RQ4</t>
+  </si>
+  <si>
+    <t>Viene verificato che sia disponibile un tutorial interattivo per la creazione delle presentazioni</t>
+  </si>
+  <si>
+    <t>RQ1
+RQ7</t>
+  </si>
+  <si>
+    <t>RQ10</t>
+  </si>
+  <si>
+    <t>Viene verificato che sia disponibile della documentazione sui test eseguiti</t>
+  </si>
+  <si>
+    <t>RQ13</t>
+  </si>
+  <si>
+    <t>Viene verificato che il sistema dovrà offrire la possibilità di eseguire offline le presentazioni</t>
+  </si>
+  <si>
+    <t>RQ16</t>
+  </si>
+  <si>
+    <t>Viene verificato che il sistema sia funzionante su dispositivi Desktop e Mobile (Android, Ios, Windows Phone)</t>
+  </si>
+  <si>
+    <t>RV1</t>
+  </si>
+  <si>
+    <t>Viene verificato che il sistema segua le linea guida del material design fornite dalla Google</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -810,17 +989,37 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color indexed="8"/>
-      <name val="Helvetica"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -850,7 +1049,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -879,13 +1078,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1189,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G105"/>
+  <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="69.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1218,615 +1423,615 @@
     </row>
     <row r="2" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>27</v>
+        <v>133</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="5"/>
+        <v>134</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>29</v>
+        <v>138</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>30</v>
+        <v>137</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="F5" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>37</v>
+        <v>139</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>38</v>
+        <v>140</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>39</v>
+        <v>141</v>
       </c>
       <c r="D7" s="4"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>41</v>
+        <v>142</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>44</v>
+        <v>147</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>45</v>
+        <v>149</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>51</v>
+        <v>150</v>
       </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>129</v>
+        <v>24</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>130</v>
+        <v>25</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>46</v>
+        <v>155</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>52</v>
+        <v>156</v>
       </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>47</v>
+        <v>157</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>53</v>
+        <v>158</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>48</v>
+        <v>159</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>54</v>
+        <v>160</v>
       </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>61</v>
+        <v>161</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>62</v>
+        <v>163</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>65</v>
+        <v>164</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>135</v>
+        <v>31</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>133</v>
+        <v>166</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>132</v>
+        <v>167</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>136</v>
+        <v>32</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>63</v>
+        <v>169</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>70</v>
+        <v>170</v>
       </c>
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>71</v>
+        <v>171</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>72</v>
+        <v>172</v>
       </c>
       <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>73</v>
+        <v>173</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>77</v>
+        <v>174</v>
       </c>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>74</v>
+        <v>175</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>78</v>
+        <v>176</v>
       </c>
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>75</v>
+        <v>177</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>79</v>
+        <v>178</v>
       </c>
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>76</v>
+        <v>179</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>80</v>
+        <v>180</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>86</v>
+        <v>181</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>90</v>
+        <v>182</v>
       </c>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>87</v>
+        <v>183</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>91</v>
+        <v>184</v>
       </c>
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>88</v>
+        <v>185</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>92</v>
+        <v>186</v>
       </c>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>89</v>
+        <v>187</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>93</v>
+        <v>188</v>
       </c>
       <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>98</v>
+        <v>189</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>104</v>
+        <v>41</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>99</v>
+        <v>190</v>
       </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>100</v>
+        <v>191</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>102</v>
+        <v>192</v>
       </c>
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>137</v>
+        <v>193</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>143</v>
+        <v>43</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>140</v>
+        <v>194</v>
       </c>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>138</v>
+        <v>195</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>144</v>
+        <v>44</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>141</v>
+        <v>196</v>
       </c>
       <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>139</v>
+        <v>197</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>145</v>
+        <v>67</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>142</v>
+        <v>198</v>
       </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>101</v>
+        <v>199</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>103</v>
+        <v>200</v>
       </c>
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
+    <row r="37" spans="1:4" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>202</v>
+      </c>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>107</v>
+        <v>203</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>119</v>
+        <v>204</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>108</v>
+        <v>205</v>
       </c>
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>114</v>
-      </c>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>110</v>
+        <v>45</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>121</v>
+        <v>57</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>115</v>
+        <v>46</v>
       </c>
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>116</v>
+        <v>47</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>112</v>
+        <v>48</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>117</v>
+        <v>53</v>
       </c>
       <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>113</v>
+        <v>49</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>124</v>
+        <v>60</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>118</v>
+        <v>54</v>
       </c>
       <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
+      <c r="A44" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>164</v>
+        <v>62</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>147</v>
+        <v>56</v>
       </c>
       <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>156</v>
-      </c>
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>149</v>
+        <v>70</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>166</v>
+        <v>84</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>157</v>
+        <v>71</v>
       </c>
       <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>167</v>
+        <v>72</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>206</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>158</v>
+        <v>78</v>
       </c>
       <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>151</v>
+        <v>73</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>168</v>
+        <v>207</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>159</v>
+        <v>79</v>
       </c>
       <c r="D49" s="4"/>
     </row>
     <row r="50" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>152</v>
+        <v>74</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>169</v>
+        <v>208</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>153</v>
+        <v>75</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>170</v>
+        <v>85</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>161</v>
+        <v>81</v>
       </c>
       <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>154</v>
+        <v>76</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>171</v>
+        <v>86</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="D52" s="4"/>
     </row>
     <row r="53" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>155</v>
+        <v>77</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>172</v>
+        <v>87</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>163</v>
+        <v>83</v>
       </c>
       <c r="D53" s="4"/>
     </row>
@@ -1838,13 +2043,13 @@
     </row>
     <row r="55" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>173</v>
+        <v>88</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>181</v>
+        <v>96</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>177</v>
+        <v>92</v>
       </c>
       <c r="D55" s="4"/>
     </row>
@@ -1856,13 +2061,13 @@
     </row>
     <row r="57" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>174</v>
+        <v>89</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>182</v>
+        <v>97</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>178</v>
+        <v>93</v>
       </c>
       <c r="D57" s="4"/>
     </row>
@@ -1874,13 +2079,13 @@
     </row>
     <row r="59" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>175</v>
+        <v>90</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>183</v>
+        <v>98</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>179</v>
+        <v>94</v>
       </c>
       <c r="D59" s="4"/>
     </row>
@@ -1892,13 +2097,13 @@
     </row>
     <row r="61" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>176</v>
+        <v>91</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>184</v>
+        <v>99</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>180</v>
+        <v>95</v>
       </c>
       <c r="D61" s="4"/>
     </row>
@@ -1910,25 +2115,25 @@
     </row>
     <row r="63" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>185</v>
+        <v>100</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>190</v>
+        <v>105</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>187</v>
+        <v>102</v>
       </c>
       <c r="D63" s="4"/>
     </row>
     <row r="64" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>186</v>
+        <v>101</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>189</v>
+        <v>104</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>188</v>
+        <v>103</v>
       </c>
       <c r="D64" s="4"/>
     </row>
@@ -1940,419 +2145,603 @@
     </row>
     <row r="66" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>191</v>
+        <v>106</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>192</v>
+        <v>107</v>
       </c>
       <c r="D66" s="4"/>
     </row>
     <row r="67" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>193</v>
+        <v>108</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>194</v>
+        <v>109</v>
       </c>
       <c r="D67" s="5"/>
     </row>
     <row r="68" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>195</v>
+        <v>110</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>196</v>
+        <v>111</v>
       </c>
       <c r="D68" s="4"/>
     </row>
     <row r="69" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="D69" s="4"/>
     </row>
     <row r="70" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>201</v>
+        <v>112</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="D70" s="4"/>
     </row>
     <row r="71" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="D71" s="4"/>
     </row>
     <row r="72" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>205</v>
-      </c>
+      <c r="A72" s="6"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
       <c r="D72" s="4"/>
     </row>
     <row r="73" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="D73" s="4"/>
     </row>
     <row r="74" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>210</v>
+        <v>9</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="D74" s="4"/>
     </row>
     <row r="75" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>213</v>
+        <v>113</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="D75" s="4"/>
     </row>
     <row r="76" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="6"/>
-      <c r="B76" s="6"/>
-      <c r="C76" s="6"/>
+      <c r="A76" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>222</v>
+      </c>
       <c r="D76" s="4"/>
     </row>
     <row r="77" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="D77" s="9"/>
+      <c r="A77" s="6"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="4"/>
     </row>
     <row r="78" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="8" t="s">
-        <v>216</v>
+      <c r="A78" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="C78" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="D78" s="9"/>
+    </row>
+    <row r="79" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C79" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="D78" s="9"/>
-    </row>
-    <row r="79" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="C79" s="8" t="s">
+      <c r="D79" s="9"/>
+    </row>
+    <row r="80" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="D79" s="9"/>
-    </row>
-    <row r="80" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="8" t="s">
-        <v>218</v>
-      </c>
       <c r="B80" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="C80" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C80" s="11" t="s">
         <v>227</v>
       </c>
       <c r="D80" s="9"/>
     </row>
     <row r="81" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="8" t="s">
-        <v>224</v>
+      <c r="A81" s="11" t="s">
+        <v>228</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="C81" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C81" s="11" t="s">
         <v>229</v>
       </c>
       <c r="D81" s="9"/>
     </row>
     <row r="82" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="8"/>
-      <c r="B82" s="8"/>
-      <c r="C82" s="8"/>
+      <c r="A82" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>231</v>
+      </c>
       <c r="D82" s="9"/>
     </row>
     <row r="83" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="8" t="s">
-        <v>230</v>
+      <c r="A83" s="11" t="s">
+        <v>233</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>214</v>
+        <v>121</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>234</v>
       </c>
       <c r="D83" s="9"/>
     </row>
     <row r="84" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="8"/>
-      <c r="C84" s="6"/>
+      <c r="C84" s="8"/>
       <c r="D84" s="9"/>
     </row>
     <row r="85" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>233</v>
+      <c r="A85" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="D85" s="9"/>
     </row>
     <row r="86" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>234</v>
-      </c>
+      <c r="A86" s="8"/>
+      <c r="B86" s="8"/>
+      <c r="C86" s="6"/>
       <c r="D86" s="9"/>
     </row>
     <row r="87" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>247</v>
+        <v>123</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>235</v>
+        <v>124</v>
       </c>
       <c r="D87" s="9"/>
     </row>
     <row r="88" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>13</v>
+        <v>129</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>236</v>
+        <v>125</v>
       </c>
       <c r="D88" s="9"/>
     </row>
     <row r="89" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>249</v>
+        <v>130</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="D89" s="10"/>
+        <v>126</v>
+      </c>
+      <c r="D89" s="9"/>
     </row>
     <row r="90" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>250</v>
+        <v>131</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="D90" s="11"/>
+        <v>127</v>
+      </c>
+      <c r="D90" s="9"/>
     </row>
     <row r="91" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D91" s="9"/>
+    </row>
+    <row r="92" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B92" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D92" s="9"/>
+    </row>
+    <row r="93" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B93" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D93" s="9"/>
+    </row>
+    <row r="94" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="D94" s="9"/>
+    </row>
+    <row r="95" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B95" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D95" s="9"/>
+    </row>
+    <row r="96" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B96" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="B91" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="D91" s="12"/>
-    </row>
-    <row r="92" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
+      <c r="C96" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="D96" s="9"/>
+    </row>
+    <row r="97" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="B92" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="D92" s="9"/>
-    </row>
-    <row r="93" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="6" t="s">
+      <c r="B97" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="C97" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="B93" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="D93" s="9"/>
-    </row>
-    <row r="94" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C94" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="D94" s="9"/>
-    </row>
-    <row r="95" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="6" t="s">
+      <c r="D97" s="9"/>
+    </row>
+    <row r="98" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B95" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="D95" s="9"/>
-    </row>
-    <row r="96" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="6" t="s">
+      <c r="B98" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C98" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="B96" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C96" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="D96" s="9"/>
-    </row>
-    <row r="97" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="B97" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="D97" s="9"/>
-    </row>
-    <row r="98" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
-      <c r="B98" s="9"/>
-      <c r="C98" s="4"/>
       <c r="D98" s="9"/>
     </row>
     <row r="99" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="9"/>
-      <c r="B99" s="9"/>
-      <c r="C99" s="4"/>
+      <c r="A99" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B99" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>259</v>
+      </c>
       <c r="D99" s="9"/>
     </row>
     <row r="100" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="9"/>
-      <c r="B100" s="9"/>
-      <c r="C100" s="4"/>
-      <c r="D100" s="9"/>
+      <c r="A100" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="101" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="9"/>
-      <c r="B101" s="9"/>
-      <c r="C101" s="4"/>
-      <c r="D101" s="9"/>
+      <c r="A101" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="102" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="9"/>
-      <c r="B102" s="9"/>
-      <c r="C102" s="4"/>
-      <c r="D102" s="9"/>
+      <c r="A102" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="103" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="9"/>
-      <c r="B103" s="9"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="9"/>
+      <c r="A103" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="104" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="9"/>
-      <c r="B104" s="9"/>
-      <c r="C104" s="4"/>
-      <c r="D104" s="9"/>
+      <c r="A104" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="105" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="9"/>
-      <c r="B105" s="9"/>
-      <c r="C105" s="4"/>
-      <c r="D105" s="9"/>
+      <c r="A105" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B120" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B122" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>315</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>